<commit_message>
- v1/welcome update - connecting to NedBank Account v4
</commit_message>
<xml_diff>
--- a/MoneyTracker/Helpers/Excel/SeedFiles/Category.xlsx
+++ b/MoneyTracker/Helpers/Excel/SeedFiles/Category.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kmadhanlala\source\repos\nedbank-money-tracker\src\Nedbank.MoneyTracker.Api\Helpers\Excel\SeedFiles\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\IQ\Projects\NedBank\Code\BitBucket\dev\nedbank-money-tracker\src\Nedbank.MoneyTracker.Api\Helpers\Excel\SeedFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FD30130-6923-428D-BD60-1DADA609C020}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -116,7 +117,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -492,11 +493,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -550,9 +551,7 @@
       <c r="E2" s="2">
         <v>1</v>
       </c>
-      <c r="G2" s="1">
-        <v>1</v>
-      </c>
+      <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
@@ -571,9 +570,7 @@
       <c r="E3" s="2">
         <v>2</v>
       </c>
-      <c r="G3" s="1">
-        <v>2</v>
-      </c>
+      <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
@@ -592,9 +589,7 @@
       <c r="E4" s="2">
         <v>1</v>
       </c>
-      <c r="G4" s="1">
-        <v>3</v>
-      </c>
+      <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
@@ -613,9 +608,7 @@
       <c r="E5" s="3">
         <v>2</v>
       </c>
-      <c r="G5" s="1">
-        <v>4</v>
-      </c>
+      <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
@@ -634,9 +627,7 @@
       <c r="E6" s="3">
         <v>1</v>
       </c>
-      <c r="G6" s="1">
-        <v>5</v>
-      </c>
+      <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
@@ -655,9 +646,7 @@
       <c r="E7" s="3">
         <v>2</v>
       </c>
-      <c r="G7" s="1">
-        <v>6</v>
-      </c>
+      <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
@@ -676,9 +665,7 @@
       <c r="E8" s="3">
         <v>1</v>
       </c>
-      <c r="G8" s="1">
-        <v>7</v>
-      </c>
+      <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
@@ -697,9 +684,7 @@
       <c r="E9" s="3">
         <v>2</v>
       </c>
-      <c r="G9" s="1">
-        <v>8</v>
-      </c>
+      <c r="G9" s="1"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
@@ -718,9 +703,7 @@
       <c r="E10" s="3">
         <v>1</v>
       </c>
-      <c r="G10" s="1">
-        <v>9</v>
-      </c>
+      <c r="G10" s="1"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="4">
@@ -736,7 +719,9 @@
       <c r="D11" s="4">
         <v>1</v>
       </c>
-      <c r="E11" s="3"/>
+      <c r="E11" s="3">
+        <v>1</v>
+      </c>
       <c r="F11" s="2">
         <v>11</v>
       </c>
@@ -758,7 +743,9 @@
       <c r="D12" s="4">
         <v>1</v>
       </c>
-      <c r="E12" s="3"/>
+      <c r="E12" s="3">
+        <v>2</v>
+      </c>
       <c r="F12" s="2">
         <v>11</v>
       </c>
@@ -780,7 +767,9 @@
       <c r="D13" s="4">
         <v>1</v>
       </c>
-      <c r="E13" s="3"/>
+      <c r="E13" s="3">
+        <v>1</v>
+      </c>
       <c r="F13" s="2">
         <v>11</v>
       </c>
@@ -802,7 +791,9 @@
       <c r="D14" s="4">
         <v>1</v>
       </c>
-      <c r="E14" s="3"/>
+      <c r="E14" s="3">
+        <v>2</v>
+      </c>
       <c r="F14" s="2">
         <v>12</v>
       </c>
@@ -824,7 +815,9 @@
       <c r="D15" s="4">
         <v>1</v>
       </c>
-      <c r="E15" s="3"/>
+      <c r="E15" s="3">
+        <v>2</v>
+      </c>
       <c r="F15" s="2">
         <v>12</v>
       </c>
@@ -846,7 +839,9 @@
       <c r="D16" s="4">
         <v>1</v>
       </c>
-      <c r="E16" s="3"/>
+      <c r="E16" s="3">
+        <v>2</v>
+      </c>
       <c r="F16" s="2">
         <v>12</v>
       </c>
@@ -868,7 +863,9 @@
       <c r="D17" s="4">
         <v>1</v>
       </c>
-      <c r="E17" s="3"/>
+      <c r="E17" s="3">
+        <v>2</v>
+      </c>
       <c r="F17" s="2">
         <v>12</v>
       </c>
@@ -893,9 +890,7 @@
       <c r="E18" s="2">
         <v>2</v>
       </c>
-      <c r="G18" s="4">
-        <v>17</v>
-      </c>
+      <c r="G18" s="4"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" s="4">
@@ -914,9 +909,7 @@
       <c r="E19" s="2">
         <v>1</v>
       </c>
-      <c r="G19" s="4">
-        <v>18</v>
-      </c>
+      <c r="G19" s="4"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" s="4">
@@ -935,9 +928,7 @@
       <c r="E20" s="2">
         <v>1</v>
       </c>
-      <c r="G20" s="4">
-        <v>19</v>
-      </c>
+      <c r="G20" s="4"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" s="4">
@@ -956,9 +947,7 @@
       <c r="E21" s="2">
         <v>2</v>
       </c>
-      <c r="G21" s="4">
-        <v>20</v>
-      </c>
+      <c r="G21" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>